<commit_message>
Guangdong update to Feb-02-00
</commit_message>
<xml_diff>
--- a/StatsWJW.xlsx
+++ b/StatsWJW.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WebSite" sheetId="3" r:id="rId1"/>
     <sheet name="Guangdong" sheetId="1" r:id="rId2"/>
-    <sheet name="Hainan" sheetId="2" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="4" r:id="rId3"/>
+    <sheet name="Hainan" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Infected</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -501,6 +502,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -563,10 +565,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Guangdong!$D$2:$D$18</c:f>
+              <c:f>Guangdong!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>19.0</c:v>
                 </c:pt>
@@ -617,16 +619,25 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Guangdong!$E$2:$E$18</c:f>
+              <c:f>Guangdong!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -677,6 +688,15 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>436.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>520.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>535.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>604.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,11 +711,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1027008512"/>
-        <c:axId val="1027012784"/>
+        <c:axId val="95136800"/>
+        <c:axId val="95140960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1027008512"/>
+        <c:axId val="95136800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,12 +771,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027012784"/>
+        <c:crossAx val="95140960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1027012784"/>
+        <c:axId val="95140960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +833,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1027008512"/>
+        <c:crossAx val="95136800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1025,11 +1045,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1026098384"/>
-        <c:axId val="1026292096"/>
+        <c:axId val="95250096"/>
+        <c:axId val="95254448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1026098384"/>
+        <c:axId val="95250096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,12 +1105,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1026292096"/>
+        <c:crossAx val="95254448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1026292096"/>
+        <c:axId val="95254448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1166,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1026098384"/>
+        <c:crossAx val="95250096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2312,15 +2332,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2642,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2988,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:E18"/>
+      <selection activeCell="E21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3045,7 +3065,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D18" si="0">B3+C3/24</f>
+        <f t="shared" ref="D3:D21" si="0">B3+C3/24</f>
         <v>21.75</v>
       </c>
       <c r="E3">
@@ -3320,6 +3340,60 @@
       </c>
       <c r="E18">
         <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <f>B19+C19/24+31</f>
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:D21" si="1">B20+C20/24+31</f>
+        <v>32.5</v>
+      </c>
+      <c r="E20">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="E21">
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -3330,6 +3404,316 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>604</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>

</xml_diff>